<commit_message>
fix: version stable de l'analyse : filtres sur les seuils fonctionnels
</commit_message>
<xml_diff>
--- a/articles_analysis.xlsx
+++ b/articles_analysis.xlsx
@@ -489,7 +489,11 @@
           <t>Soins (Type: OTHER, Saillance: 0.68) | Cosmétiques Bio (Type: CONSUMER_GOOD, Saillance: 0.32)</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>/Beauty &amp; Fitness (Confidence: 0.63)</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix: version stable de l'analyse : feedback sur l'ui pour l'UX
</commit_message>
<xml_diff>
--- a/articles_analysis.xlsx
+++ b/articles_analysis.xlsx
@@ -466,11 +466,7 @@
           <t>Rétinol-Like Végétal : l'alternative antirides high-tech et naturelle</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Rétinol (Type: OTHER, Saillance: 0.36) | high-tech (Type: OTHER, Saillance: 0.32) | Like Végétal (Type: OTHER, Saillance: 0.18) | alternative (Type: OTHER, Saillance: 0.14)</t>
-        </is>
-      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -484,16 +480,8 @@
           <t>Soins Cosmétiques Bio</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Soins (Type: OTHER, Saillance: 0.68) | Cosmétiques Bio (Type: CONSUMER_GOOD, Saillance: 0.32)</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>/Beauty &amp; Fitness (Confidence: 0.63)</t>
-        </is>
-      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>